<commit_message>
Changes in structure and progress in forms
</commit_message>
<xml_diff>
--- a/src/data/dato.xlsx
+++ b/src/data/dato.xlsx
@@ -420,15 +420,7 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Progress in the implementation in the view of a movie
</commit_message>
<xml_diff>
--- a/src/data/dato.xlsx
+++ b/src/data/dato.xlsx
@@ -420,15 +420,7 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>